<commit_message>
Finalización de la cuenta
</commit_message>
<xml_diff>
--- a/datos/CLASIFICACIONES.xlsx
+++ b/datos/CLASIFICACIONES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renato\GitHub\scn_scae_gt\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AD18C0-1936-43C8-8A1E-229BE607C8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2402F5-C87C-411C-BBF5-C50AAC216265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{C22BA8DC-7785-47D2-AF50-A04A94E3F417}"/>
+    <workbookView xWindow="743" yWindow="-98" windowWidth="18555" windowHeight="10996" activeTab="4" xr2:uid="{C22BA8DC-7785-47D2-AF50-A04A94E3F417}"/>
   </bookViews>
   <sheets>
     <sheet name="columnas" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4075" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="1484">
   <si>
     <t>P0101</t>
   </si>
@@ -4470,6 +4470,39 @@
   </si>
   <si>
     <t>N2O equivalente</t>
+  </si>
+  <si>
+    <t>GTMva000</t>
+  </si>
+  <si>
+    <t>Valor agregado</t>
+  </si>
+  <si>
+    <t>Valor Agregado</t>
+  </si>
+  <si>
+    <t>Energía eléctrica, gas, vapor y aire acondicionado</t>
+  </si>
+  <si>
+    <t>Otras primarias (incluye solar)</t>
+  </si>
+  <si>
+    <t>id_ciiu1_compacta</t>
+  </si>
+  <si>
+    <t>ciiu1_compacta</t>
+  </si>
+  <si>
+    <t>No determinada</t>
+  </si>
+  <si>
+    <t>I-S</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>D-E</t>
   </si>
 </sst>
 </file>
@@ -4848,8 +4881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{929882BB-EC53-415D-8756-EE638CA8DF7A}">
   <dimension ref="A1:C339"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8374,10 +8407,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186748BD-FE1A-4F85-84AF-EE7AA794CE26}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8431,6 +8464,14 @@
       </c>
       <c r="B6" t="s">
         <v>1397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1474</v>
       </c>
     </row>
   </sheetData>
@@ -34299,10 +34340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630F3B5A-7724-4218-8CEA-54B103D0974A}">
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
-    <sheetView topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A227" sqref="A227:A229"/>
+    <sheetView topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36787,6 +36828,14 @@
         <v>1403</v>
       </c>
     </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A230" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B230">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36795,10 +36844,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DC7725-521A-47B8-B2E7-57FAA2BB5224}">
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C229" sqref="C229"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="A230" sqref="A230:C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39283,6 +39332,14 @@
         <v>1403</v>
       </c>
     </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A230" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B230">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39292,7 +39349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05E38F5-79ED-4AF1-BD6D-0CBD9E0C28A7}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -40139,10 +40196,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E379736E-AEF6-4880-BCC8-DFD07670FC02}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -40150,7 +40207,7 @@
     <col min="2" max="2" width="32.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>785</v>
       </c>
@@ -40166,8 +40223,14 @@
       <c r="E1" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>437</v>
       </c>
@@ -40183,8 +40246,16 @@
       <c r="E2" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="str">
+        <f>VLOOKUP(C2,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G2" t="str">
+        <f>VLOOKUP(C2,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>438</v>
       </c>
@@ -40200,8 +40271,16 @@
       <c r="E3" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="str">
+        <f>VLOOKUP(C3,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(C3,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>440</v>
       </c>
@@ -40217,8 +40296,16 @@
       <c r="E4" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="str">
+        <f>VLOOKUP(C4,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(C4,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>441</v>
       </c>
@@ -40234,8 +40321,16 @@
       <c r="E5" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="str">
+        <f>VLOOKUP(C5,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(C5,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>443</v>
       </c>
@@ -40251,8 +40346,16 @@
       <c r="E6" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="str">
+        <f>VLOOKUP(C6,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(C6,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>444</v>
       </c>
@@ -40268,8 +40371,16 @@
       <c r="E7" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7" t="str">
+        <f>VLOOKUP(C7,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(C7,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>446</v>
       </c>
@@ -40285,8 +40396,16 @@
       <c r="E8" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" t="str">
+        <f>VLOOKUP(C8,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(C8,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>448</v>
       </c>
@@ -40302,8 +40421,16 @@
       <c r="E9" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" t="str">
+        <f>VLOOKUP(C9,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(C9,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>449</v>
       </c>
@@ -40319,8 +40446,16 @@
       <c r="E10" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" t="str">
+        <f>VLOOKUP(C10,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(C10,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>451</v>
       </c>
@@ -40336,8 +40471,16 @@
       <c r="E11" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11" t="str">
+        <f>VLOOKUP(C11,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(C11,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>453</v>
       </c>
@@ -40353,8 +40496,16 @@
       <c r="E12" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="str">
+        <f>VLOOKUP(C12,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(C12,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>454</v>
       </c>
@@ -40370,8 +40521,16 @@
       <c r="E13" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13" t="str">
+        <f>VLOOKUP(C13,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(C13,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>455</v>
       </c>
@@ -40387,8 +40546,16 @@
       <c r="E14" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="str">
+        <f>VLOOKUP(C14,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(C14,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>457</v>
       </c>
@@ -40404,8 +40571,16 @@
       <c r="E15" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F15" t="str">
+        <f>VLOOKUP(C15,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(C15,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>458</v>
       </c>
@@ -40421,8 +40596,16 @@
       <c r="E16" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="str">
+        <f>VLOOKUP(C16,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(C16,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>459</v>
       </c>
@@ -40438,8 +40621,16 @@
       <c r="E17" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="str">
+        <f>VLOOKUP(C17,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(C17,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>460</v>
       </c>
@@ -40455,8 +40646,16 @@
       <c r="E18" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="str">
+        <f>VLOOKUP(C18,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(C18,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>461</v>
       </c>
@@ -40472,8 +40671,16 @@
       <c r="E19" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="str">
+        <f>VLOOKUP(C19,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(C19,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>463</v>
       </c>
@@ -40489,8 +40696,16 @@
       <c r="E20" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="str">
+        <f>VLOOKUP(C20,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(C20,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>465</v>
       </c>
@@ -40506,8 +40721,16 @@
       <c r="E21" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" t="str">
+        <f>VLOOKUP(C21,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP(C21,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>466</v>
       </c>
@@ -40523,8 +40746,16 @@
       <c r="E22" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" t="str">
+        <f>VLOOKUP(C22,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(C22,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>468</v>
       </c>
@@ -40540,8 +40771,16 @@
       <c r="E23" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" t="str">
+        <f>VLOOKUP(C23,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(C23,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>469</v>
       </c>
@@ -40557,8 +40796,16 @@
       <c r="E24" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="str">
+        <f>VLOOKUP(C24,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(C24,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Agricultura</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>471</v>
       </c>
@@ -40574,8 +40821,16 @@
       <c r="E25" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25" t="str">
+        <f>VLOOKUP(C25,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(C25,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Minería</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>473</v>
       </c>
@@ -40591,8 +40846,16 @@
       <c r="E26" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26" t="str">
+        <f>VLOOKUP(C26,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP(C26,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Minería</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>475</v>
       </c>
@@ -40608,8 +40871,16 @@
       <c r="E27" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F27" t="str">
+        <f>VLOOKUP(C27,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(C27,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Minería</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>477</v>
       </c>
@@ -40625,8 +40896,16 @@
       <c r="E28" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F28" t="str">
+        <f>VLOOKUP(C28,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="G28" t="str">
+        <f>VLOOKUP(C28,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Minería</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>479</v>
       </c>
@@ -40642,8 +40921,16 @@
       <c r="E29" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F29" t="str">
+        <f>VLOOKUP(C29,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>B</v>
+      </c>
+      <c r="G29" t="str">
+        <f>VLOOKUP(C29,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Minería</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>481</v>
       </c>
@@ -40659,8 +40946,16 @@
       <c r="E30" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F30" t="str">
+        <f>VLOOKUP(C30,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G30" t="str">
+        <f>VLOOKUP(C30,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>483</v>
       </c>
@@ -40676,8 +40971,16 @@
       <c r="E31" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F31" t="str">
+        <f>VLOOKUP(C31,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G31" t="str">
+        <f>VLOOKUP(C31,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>484</v>
       </c>
@@ -40693,8 +40996,16 @@
       <c r="E32" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F32" t="str">
+        <f>VLOOKUP(C32,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G32" t="str">
+        <f>VLOOKUP(C32,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>486</v>
       </c>
@@ -40710,8 +41021,16 @@
       <c r="E33" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F33" t="str">
+        <f>VLOOKUP(C33,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G33" t="str">
+        <f>VLOOKUP(C33,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>488</v>
       </c>
@@ -40727,8 +41046,16 @@
       <c r="E34" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F34" t="str">
+        <f>VLOOKUP(C34,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G34" t="str">
+        <f>VLOOKUP(C34,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>490</v>
       </c>
@@ -40744,8 +41071,16 @@
       <c r="E35" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" t="str">
+        <f>VLOOKUP(C35,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G35" t="str">
+        <f>VLOOKUP(C35,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>491</v>
       </c>
@@ -40761,8 +41096,16 @@
       <c r="E36" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F36" t="str">
+        <f>VLOOKUP(C36,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G36" t="str">
+        <f>VLOOKUP(C36,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>493</v>
       </c>
@@ -40778,8 +41121,16 @@
       <c r="E37" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37" t="str">
+        <f>VLOOKUP(C37,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G37" t="str">
+        <f>VLOOKUP(C37,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>494</v>
       </c>
@@ -40795,8 +41146,16 @@
       <c r="E38" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F38" t="str">
+        <f>VLOOKUP(C38,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G38" t="str">
+        <f>VLOOKUP(C38,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>495</v>
       </c>
@@ -40812,8 +41171,16 @@
       <c r="E39" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F39" t="str">
+        <f>VLOOKUP(C39,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G39" t="str">
+        <f>VLOOKUP(C39,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>496</v>
       </c>
@@ -40829,8 +41196,16 @@
       <c r="E40" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F40" t="str">
+        <f>VLOOKUP(C40,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G40" t="str">
+        <f>VLOOKUP(C40,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>498</v>
       </c>
@@ -40846,8 +41221,16 @@
       <c r="E41" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F41" t="str">
+        <f>VLOOKUP(C41,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G41" t="str">
+        <f>VLOOKUP(C41,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>499</v>
       </c>
@@ -40863,8 +41246,16 @@
       <c r="E42" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42" t="str">
+        <f>VLOOKUP(C42,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G42" t="str">
+        <f>VLOOKUP(C42,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>500</v>
       </c>
@@ -40880,8 +41271,16 @@
       <c r="E43" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F43" t="str">
+        <f>VLOOKUP(C43,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G43" t="str">
+        <f>VLOOKUP(C43,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>502</v>
       </c>
@@ -40897,8 +41296,16 @@
       <c r="E44" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F44" t="str">
+        <f>VLOOKUP(C44,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G44" t="str">
+        <f>VLOOKUP(C44,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>503</v>
       </c>
@@ -40914,8 +41321,16 @@
       <c r="E45" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F45" t="str">
+        <f>VLOOKUP(C45,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G45" t="str">
+        <f>VLOOKUP(C45,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>504</v>
       </c>
@@ -40931,8 +41346,16 @@
       <c r="E46" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F46" t="str">
+        <f>VLOOKUP(C46,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G46" t="str">
+        <f>VLOOKUP(C46,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>506</v>
       </c>
@@ -40948,8 +41371,16 @@
       <c r="E47" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F47" t="str">
+        <f>VLOOKUP(C47,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G47" t="str">
+        <f>VLOOKUP(C47,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>508</v>
       </c>
@@ -40965,8 +41396,16 @@
       <c r="E48" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F48" t="str">
+        <f>VLOOKUP(C48,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G48" t="str">
+        <f>VLOOKUP(C48,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>509</v>
       </c>
@@ -40982,8 +41421,16 @@
       <c r="E49" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F49" t="str">
+        <f>VLOOKUP(C49,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G49" t="str">
+        <f>VLOOKUP(C49,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>510</v>
       </c>
@@ -40999,8 +41446,16 @@
       <c r="E50" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F50" t="str">
+        <f>VLOOKUP(C50,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G50" t="str">
+        <f>VLOOKUP(C50,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>512</v>
       </c>
@@ -41016,8 +41471,16 @@
       <c r="E51" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51" t="str">
+        <f>VLOOKUP(C51,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G51" t="str">
+        <f>VLOOKUP(C51,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>513</v>
       </c>
@@ -41033,8 +41496,16 @@
       <c r="E52" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52" t="str">
+        <f>VLOOKUP(C52,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G52" t="str">
+        <f>VLOOKUP(C52,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>515</v>
       </c>
@@ -41050,8 +41521,16 @@
       <c r="E53" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" t="str">
+        <f>VLOOKUP(C53,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G53" t="str">
+        <f>VLOOKUP(C53,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>516</v>
       </c>
@@ -41067,8 +41546,16 @@
       <c r="E54" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54" t="str">
+        <f>VLOOKUP(C54,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G54" t="str">
+        <f>VLOOKUP(C54,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>518</v>
       </c>
@@ -41084,8 +41571,16 @@
       <c r="E55" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55" t="str">
+        <f>VLOOKUP(C55,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G55" t="str">
+        <f>VLOOKUP(C55,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>520</v>
       </c>
@@ -41101,8 +41596,16 @@
       <c r="E56" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" t="str">
+        <f>VLOOKUP(C56,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G56" t="str">
+        <f>VLOOKUP(C56,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>522</v>
       </c>
@@ -41118,8 +41621,16 @@
       <c r="E57" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57" t="str">
+        <f>VLOOKUP(C57,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G57" t="str">
+        <f>VLOOKUP(C57,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>524</v>
       </c>
@@ -41135,8 +41646,16 @@
       <c r="E58" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58" t="str">
+        <f>VLOOKUP(C58,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G58" t="str">
+        <f>VLOOKUP(C58,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>525</v>
       </c>
@@ -41152,8 +41671,16 @@
       <c r="E59" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59" t="str">
+        <f>VLOOKUP(C59,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G59" t="str">
+        <f>VLOOKUP(C59,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>526</v>
       </c>
@@ -41169,8 +41696,16 @@
       <c r="E60" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60" t="str">
+        <f>VLOOKUP(C60,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G60" t="str">
+        <f>VLOOKUP(C60,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>527</v>
       </c>
@@ -41186,8 +41721,16 @@
       <c r="E61" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61" t="str">
+        <f>VLOOKUP(C61,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G61" t="str">
+        <f>VLOOKUP(C61,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>529</v>
       </c>
@@ -41203,8 +41746,16 @@
       <c r="E62" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F62" t="str">
+        <f>VLOOKUP(C62,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G62" t="str">
+        <f>VLOOKUP(C62,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>531</v>
       </c>
@@ -41220,8 +41771,16 @@
       <c r="E63" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F63" t="str">
+        <f>VLOOKUP(C63,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G63" t="str">
+        <f>VLOOKUP(C63,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>533</v>
       </c>
@@ -41237,8 +41796,16 @@
       <c r="E64" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F64" t="str">
+        <f>VLOOKUP(C64,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G64" t="str">
+        <f>VLOOKUP(C64,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>534</v>
       </c>
@@ -41254,8 +41821,16 @@
       <c r="E65" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F65" t="str">
+        <f>VLOOKUP(C65,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G65" t="str">
+        <f>VLOOKUP(C65,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>536</v>
       </c>
@@ -41271,8 +41846,16 @@
       <c r="E66" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66" t="str">
+        <f>VLOOKUP(C66,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G66" t="str">
+        <f>VLOOKUP(C66,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>538</v>
       </c>
@@ -41288,8 +41871,16 @@
       <c r="E67" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F67" t="str">
+        <f>VLOOKUP(C67,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G67" t="str">
+        <f>VLOOKUP(C67,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>540</v>
       </c>
@@ -41305,8 +41896,16 @@
       <c r="E68" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F68" t="str">
+        <f>VLOOKUP(C68,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G68" t="str">
+        <f>VLOOKUP(C68,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>541</v>
       </c>
@@ -41322,8 +41921,16 @@
       <c r="E69" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F69" t="str">
+        <f>VLOOKUP(C69,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G69" t="str">
+        <f>VLOOKUP(C69,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>542</v>
       </c>
@@ -41339,8 +41946,16 @@
       <c r="E70" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F70" t="str">
+        <f>VLOOKUP(C70,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G70" t="str">
+        <f>VLOOKUP(C70,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>544</v>
       </c>
@@ -41356,8 +41971,16 @@
       <c r="E71" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71" t="str">
+        <f>VLOOKUP(C71,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G71" t="str">
+        <f>VLOOKUP(C71,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>545</v>
       </c>
@@ -41373,8 +41996,16 @@
       <c r="E72" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F72" t="str">
+        <f>VLOOKUP(C72,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G72" t="str">
+        <f>VLOOKUP(C72,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>547</v>
       </c>
@@ -41390,8 +42021,16 @@
       <c r="E73" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F73" t="str">
+        <f>VLOOKUP(C73,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G73" t="str">
+        <f>VLOOKUP(C73,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>549</v>
       </c>
@@ -41407,8 +42046,16 @@
       <c r="E74" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F74" t="str">
+        <f>VLOOKUP(C74,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G74" t="str">
+        <f>VLOOKUP(C74,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>551</v>
       </c>
@@ -41424,8 +42071,16 @@
       <c r="E75" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F75" t="str">
+        <f>VLOOKUP(C75,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G75" t="str">
+        <f>VLOOKUP(C75,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>552</v>
       </c>
@@ -41441,8 +42096,16 @@
       <c r="E76" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F76" t="str">
+        <f>VLOOKUP(C76,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G76" t="str">
+        <f>VLOOKUP(C76,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>554</v>
       </c>
@@ -41458,8 +42121,16 @@
       <c r="E77" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F77" t="str">
+        <f>VLOOKUP(C77,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G77" t="str">
+        <f>VLOOKUP(C77,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>556</v>
       </c>
@@ -41475,8 +42146,16 @@
       <c r="E78" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F78" t="str">
+        <f>VLOOKUP(C78,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G78" t="str">
+        <f>VLOOKUP(C78,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>557</v>
       </c>
@@ -41492,8 +42171,16 @@
       <c r="E79" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F79" t="str">
+        <f>VLOOKUP(C79,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G79" t="str">
+        <f>VLOOKUP(C79,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>558</v>
       </c>
@@ -41509,8 +42196,16 @@
       <c r="E80" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F80" t="str">
+        <f>VLOOKUP(C80,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G80" t="str">
+        <f>VLOOKUP(C80,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>560</v>
       </c>
@@ -41526,8 +42221,16 @@
       <c r="E81" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F81" t="str">
+        <f>VLOOKUP(C81,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G81" t="str">
+        <f>VLOOKUP(C81,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>561</v>
       </c>
@@ -41543,8 +42246,16 @@
       <c r="E82" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F82" t="str">
+        <f>VLOOKUP(C82,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>C</v>
+      </c>
+      <c r="G82" t="str">
+        <f>VLOOKUP(C82,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Manufacturas</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>563</v>
       </c>
@@ -41560,8 +42271,16 @@
       <c r="E83" t="s">
         <v>1454</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F83" t="str">
+        <f>VLOOKUP(C83,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>D-E</v>
+      </c>
+      <c r="G83" t="str">
+        <f>VLOOKUP(C83,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Servicios básicos</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>565</v>
       </c>
@@ -41577,8 +42296,16 @@
       <c r="E84" t="s">
         <v>1455</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F84" t="str">
+        <f>VLOOKUP(C84,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>D-E</v>
+      </c>
+      <c r="G84" t="str">
+        <f>VLOOKUP(C84,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Servicios básicos</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>567</v>
       </c>
@@ -41594,8 +42321,16 @@
       <c r="E85" t="s">
         <v>1455</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F85" t="str">
+        <f>VLOOKUP(C85,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>D-E</v>
+      </c>
+      <c r="G85" t="str">
+        <f>VLOOKUP(C85,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Servicios básicos</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>568</v>
       </c>
@@ -41611,8 +42346,16 @@
       <c r="E86" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F86" t="str">
+        <f>VLOOKUP(C86,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>F</v>
+      </c>
+      <c r="G86" t="str">
+        <f>VLOOKUP(C86,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Construcción</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>570</v>
       </c>
@@ -41628,8 +42371,16 @@
       <c r="E87" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F87" t="str">
+        <f>VLOOKUP(C87,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>F</v>
+      </c>
+      <c r="G87" t="str">
+        <f>VLOOKUP(C87,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Construcción</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>571</v>
       </c>
@@ -41645,8 +42396,16 @@
       <c r="E88" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F88" t="str">
+        <f>VLOOKUP(C88,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>F</v>
+      </c>
+      <c r="G88" t="str">
+        <f>VLOOKUP(C88,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Construcción</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>572</v>
       </c>
@@ -41662,8 +42421,16 @@
       <c r="E89" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F89" t="str">
+        <f>VLOOKUP(C89,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>G</v>
+      </c>
+      <c r="G89" t="str">
+        <f>VLOOKUP(C89,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Comercio</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>573</v>
       </c>
@@ -41679,8 +42446,16 @@
       <c r="E90" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F90" t="str">
+        <f>VLOOKUP(C90,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>G</v>
+      </c>
+      <c r="G90" t="str">
+        <f>VLOOKUP(C90,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Comercio</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>574</v>
       </c>
@@ -41696,8 +42471,16 @@
       <c r="E91" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F91" t="str">
+        <f>VLOOKUP(C91,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>H</v>
+      </c>
+      <c r="G91" t="str">
+        <f>VLOOKUP(C91,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Transporte</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>575</v>
       </c>
@@ -41713,8 +42496,16 @@
       <c r="E92" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F92" t="str">
+        <f>VLOOKUP(C92,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>H</v>
+      </c>
+      <c r="G92" t="str">
+        <f>VLOOKUP(C92,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Transporte</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>576</v>
       </c>
@@ -41730,8 +42521,16 @@
       <c r="E93" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F93" t="str">
+        <f>VLOOKUP(C93,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>H</v>
+      </c>
+      <c r="G93" t="str">
+        <f>VLOOKUP(C93,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Transporte</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>577</v>
       </c>
@@ -41747,8 +42546,16 @@
       <c r="E94" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F94" t="str">
+        <f>VLOOKUP(C94,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G94" t="str">
+        <f>VLOOKUP(C94,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>578</v>
       </c>
@@ -41764,8 +42571,16 @@
       <c r="E95" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F95" t="str">
+        <f>VLOOKUP(C95,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G95" t="str">
+        <f>VLOOKUP(C95,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>579</v>
       </c>
@@ -41781,8 +42596,16 @@
       <c r="E96" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F96" t="str">
+        <f>VLOOKUP(C96,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G96" t="str">
+        <f>VLOOKUP(C96,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>580</v>
       </c>
@@ -41798,8 +42621,16 @@
       <c r="E97" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F97" t="str">
+        <f>VLOOKUP(C97,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G97" t="str">
+        <f>VLOOKUP(C97,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>581</v>
       </c>
@@ -41815,8 +42646,16 @@
       <c r="E98" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F98" t="str">
+        <f>VLOOKUP(C98,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G98" t="str">
+        <f>VLOOKUP(C98,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>582</v>
       </c>
@@ -41832,8 +42671,16 @@
       <c r="E99" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F99" t="str">
+        <f>VLOOKUP(C99,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G99" t="str">
+        <f>VLOOKUP(C99,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>583</v>
       </c>
@@ -41849,8 +42696,16 @@
       <c r="E100" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F100" t="str">
+        <f>VLOOKUP(C100,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G100" t="str">
+        <f>VLOOKUP(C100,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>584</v>
       </c>
@@ -41866,8 +42721,16 @@
       <c r="E101" t="s">
         <v>1458</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F101" t="str">
+        <f>VLOOKUP(C101,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G101" t="str">
+        <f>VLOOKUP(C101,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>585</v>
       </c>
@@ -41883,8 +42746,16 @@
       <c r="E102" t="s">
         <v>1458</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F102" t="str">
+        <f>VLOOKUP(C102,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G102" t="str">
+        <f>VLOOKUP(C102,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>586</v>
       </c>
@@ -41900,8 +42771,16 @@
       <c r="E103" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F103" t="str">
+        <f>VLOOKUP(C103,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G103" t="str">
+        <f>VLOOKUP(C103,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>587</v>
       </c>
@@ -41917,8 +42796,16 @@
       <c r="E104" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F104" t="str">
+        <f>VLOOKUP(C104,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G104" t="str">
+        <f>VLOOKUP(C104,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>588</v>
       </c>
@@ -41934,8 +42821,16 @@
       <c r="E105" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F105" t="str">
+        <f>VLOOKUP(C105,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G105" t="str">
+        <f>VLOOKUP(C105,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>589</v>
       </c>
@@ -41951,8 +42846,16 @@
       <c r="E106" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F106" t="str">
+        <f>VLOOKUP(C106,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G106" t="str">
+        <f>VLOOKUP(C106,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>591</v>
       </c>
@@ -41968,8 +42871,16 @@
       <c r="E107" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F107" t="str">
+        <f>VLOOKUP(C107,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G107" t="str">
+        <f>VLOOKUP(C107,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>592</v>
       </c>
@@ -41985,8 +42896,16 @@
       <c r="E108" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F108" t="str">
+        <f>VLOOKUP(C108,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G108" t="str">
+        <f>VLOOKUP(C108,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>692</v>
       </c>
@@ -42002,8 +42921,16 @@
       <c r="E109" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F109" t="str">
+        <f>VLOOKUP(C109,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G109" t="str">
+        <f>VLOOKUP(C109,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>593</v>
       </c>
@@ -42019,8 +42946,16 @@
       <c r="E110" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F110" t="str">
+        <f>VLOOKUP(C110,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G110" t="str">
+        <f>VLOOKUP(C110,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>594</v>
       </c>
@@ -42036,8 +42971,16 @@
       <c r="E111" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F111" t="str">
+        <f>VLOOKUP(C111,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G111" t="str">
+        <f>VLOOKUP(C111,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>595</v>
       </c>
@@ -42053,8 +42996,16 @@
       <c r="E112" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F112" t="str">
+        <f>VLOOKUP(C112,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G112" t="str">
+        <f>VLOOKUP(C112,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>596</v>
       </c>
@@ -42070,8 +43021,16 @@
       <c r="E113" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F113" t="str">
+        <f>VLOOKUP(C113,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G113" t="str">
+        <f>VLOOKUP(C113,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>597</v>
       </c>
@@ -42087,8 +43046,16 @@
       <c r="E114" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F114" t="str">
+        <f>VLOOKUP(C114,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G114" t="str">
+        <f>VLOOKUP(C114,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>598</v>
       </c>
@@ -42104,8 +43071,16 @@
       <c r="E115" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F115" t="str">
+        <f>VLOOKUP(C115,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G115" t="str">
+        <f>VLOOKUP(C115,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>599</v>
       </c>
@@ -42121,8 +43096,16 @@
       <c r="E116" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F116" t="str">
+        <f>VLOOKUP(C116,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G116" t="str">
+        <f>VLOOKUP(C116,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>600</v>
       </c>
@@ -42138,8 +43121,16 @@
       <c r="E117" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F117" t="str">
+        <f>VLOOKUP(C117,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G117" t="str">
+        <f>VLOOKUP(C117,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>601</v>
       </c>
@@ -42155,8 +43146,16 @@
       <c r="E118" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F118" t="str">
+        <f>VLOOKUP(C118,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G118" t="str">
+        <f>VLOOKUP(C118,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>602</v>
       </c>
@@ -42172,8 +43171,16 @@
       <c r="E119" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F119" t="str">
+        <f>VLOOKUP(C119,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G119" t="str">
+        <f>VLOOKUP(C119,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>693</v>
       </c>
@@ -42189,8 +43196,16 @@
       <c r="E120" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F120" t="str">
+        <f>VLOOKUP(C120,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G120" t="str">
+        <f>VLOOKUP(C120,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>694</v>
       </c>
@@ -42206,8 +43221,16 @@
       <c r="E121" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F121" t="str">
+        <f>VLOOKUP(C121,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G121" t="str">
+        <f>VLOOKUP(C121,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>695</v>
       </c>
@@ -42223,8 +43246,16 @@
       <c r="E122" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F122" t="str">
+        <f>VLOOKUP(C122,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G122" t="str">
+        <f>VLOOKUP(C122,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>696</v>
       </c>
@@ -42240,8 +43271,16 @@
       <c r="E123" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F123" t="str">
+        <f>VLOOKUP(C123,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G123" t="str">
+        <f>VLOOKUP(C123,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>697</v>
       </c>
@@ -42257,8 +43296,16 @@
       <c r="E124" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F124" t="str">
+        <f>VLOOKUP(C124,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G124" t="str">
+        <f>VLOOKUP(C124,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>698</v>
       </c>
@@ -42274,8 +43321,16 @@
       <c r="E125" t="s">
         <v>1463</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F125" t="str">
+        <f>VLOOKUP(C125,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G125" t="str">
+        <f>VLOOKUP(C125,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>699</v>
       </c>
@@ -42291,8 +43346,16 @@
       <c r="E126" t="s">
         <v>1463</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F126" t="str">
+        <f>VLOOKUP(C126,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G126" t="str">
+        <f>VLOOKUP(C126,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>603</v>
       </c>
@@ -42308,8 +43371,16 @@
       <c r="E127" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F127" t="str">
+        <f>VLOOKUP(C127,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G127" t="str">
+        <f>VLOOKUP(C127,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>604</v>
       </c>
@@ -42325,8 +43396,16 @@
       <c r="E128" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F128" t="str">
+        <f>VLOOKUP(C128,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G128" t="str">
+        <f>VLOOKUP(C128,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>605</v>
       </c>
@@ -42342,8 +43421,16 @@
       <c r="E129" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F129" t="str">
+        <f>VLOOKUP(C129,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G129" t="str">
+        <f>VLOOKUP(C129,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>606</v>
       </c>
@@ -42359,8 +43446,16 @@
       <c r="E130" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F130" t="str">
+        <f>VLOOKUP(C130,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G130" t="str">
+        <f>VLOOKUP(C130,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>607</v>
       </c>
@@ -42376,8 +43471,16 @@
       <c r="E131" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F131" t="str">
+        <f>VLOOKUP(C131,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G131" t="str">
+        <f>VLOOKUP(C131,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>608</v>
       </c>
@@ -42393,8 +43496,16 @@
       <c r="E132" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F132" t="str">
+        <f>VLOOKUP(C132,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G132" t="str">
+        <f>VLOOKUP(C132,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>609</v>
       </c>
@@ -42410,8 +43521,16 @@
       <c r="E133" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F133" t="str">
+        <f>VLOOKUP(C133,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>I-S</v>
+      </c>
+      <c r="G133" t="str">
+        <f>VLOOKUP(C133,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>Otros servicios</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>1378</v>
       </c>
@@ -42426,6 +43545,14 @@
       </c>
       <c r="E134" t="s">
         <v>1382</v>
+      </c>
+      <c r="F134" t="str">
+        <f>VLOOKUP(C134,ciiu!$A$2:$E$22,4,FALSE)</f>
+        <v>Z</v>
+      </c>
+      <c r="G134" t="str">
+        <f>VLOOKUP(C134,ciiu!$A$2:$E$22,5,FALSE)</f>
+        <v>No determinada</v>
       </c>
     </row>
   </sheetData>
@@ -42435,10 +43562,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64B7F33-8442-4A7B-9699-879DCF816A72}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -42446,7 +43573,7 @@
     <col min="2" max="2" width="23.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1448</v>
       </c>
@@ -42456,8 +43583,14 @@
       <c r="C1" t="s">
         <v>1450</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1410</v>
       </c>
@@ -42467,8 +43600,14 @@
       <c r="C2" t="s">
         <v>1451</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1412</v>
       </c>
@@ -42478,8 +43617,14 @@
       <c r="C3" t="s">
         <v>1452</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1414</v>
       </c>
@@ -42489,8 +43634,14 @@
       <c r="C4" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1416</v>
       </c>
@@ -42500,8 +43651,14 @@
       <c r="C5" t="s">
         <v>1454</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1388</v>
       </c>
@@ -42511,8 +43668,14 @@
       <c r="C6" t="s">
         <v>1455</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1418</v>
       </c>
@@ -42522,8 +43685,14 @@
       <c r="C7" t="s">
         <v>1419</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1420</v>
       </c>
@@ -42533,8 +43702,14 @@
       <c r="C8" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>1420</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1422</v>
       </c>
@@ -42544,8 +43719,14 @@
       <c r="C9" t="s">
         <v>1423</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1424</v>
       </c>
@@ -42555,8 +43736,14 @@
       <c r="C10" t="s">
         <v>1425</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1426</v>
       </c>
@@ -42566,8 +43753,14 @@
       <c r="C11" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1428</v>
       </c>
@@ -42577,8 +43770,14 @@
       <c r="C12" t="s">
         <v>1458</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E12" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>1430</v>
       </c>
@@ -42588,8 +43787,14 @@
       <c r="C13" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>1432</v>
       </c>
@@ -42599,8 +43804,14 @@
       <c r="C14" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E14" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>1434</v>
       </c>
@@ -42610,8 +43821,14 @@
       <c r="C15" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>1436</v>
       </c>
@@ -42621,8 +43838,14 @@
       <c r="C16" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E16" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>1437</v>
       </c>
@@ -42632,8 +43855,14 @@
       <c r="C17" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E17" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>1439</v>
       </c>
@@ -42643,8 +43872,14 @@
       <c r="C18" t="s">
         <v>1463</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E18" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>1441</v>
       </c>
@@ -42654,8 +43889,14 @@
       <c r="C19" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E19" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>1443</v>
       </c>
@@ -42665,8 +43906,14 @@
       <c r="C20" t="s">
         <v>1464</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>1445</v>
       </c>
@@ -42676,8 +43923,14 @@
       <c r="C21" t="s">
         <v>1465</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E21" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>1449</v>
       </c>
@@ -42686,6 +43939,12 @@
       </c>
       <c r="C22" t="s">
         <v>1382</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1480</v>
       </c>
     </row>
   </sheetData>
@@ -42697,8 +43956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D1C4B1-99FA-4847-8C6B-549B844D73AF}">
   <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="B222" sqref="B222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -44273,7 +45532,7 @@
         <v>282</v>
       </c>
       <c r="B143" t="s">
-        <v>283</v>
+        <v>1476</v>
       </c>
       <c r="C143" s="1">
         <v>3</v>
@@ -45131,7 +46390,7 @@
         <v>1403</v>
       </c>
       <c r="B221" t="s">
-        <v>1408</v>
+        <v>1477</v>
       </c>
       <c r="C221" s="1">
         <v>2</v>
@@ -45245,10 +46504,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE949D2-F99D-4CAF-85D0-EEE8FDE4F5CB}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -45333,6 +46592,14 @@
         <v>1472</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1475</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>